<commit_message>
Updating parameters used for SOM
</commit_message>
<xml_diff>
--- a/data/somParams/params_SOM.xlsx
+++ b/data/somParams/params_SOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustinkincaid/Google Drive/2_UVM/MansfieldHydro/data/somParams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E435BC56-9124-C64D-AF93-DC86CF8B9720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AA4E94-33A1-5142-B90F-366F420B8F87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="860" windowWidth="22820" windowHeight="16660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="860" windowWidth="22820" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="full" sheetId="10" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="21">
   <si>
     <t>myRun</t>
   </si>
@@ -89,6 +89,12 @@
   <si>
     <t>205 Vesanto nodes</t>
   </si>
+  <si>
+    <t>1.3 ratio of cols to rows</t>
+  </si>
+  <si>
+    <t>175 Vesanto nodes</t>
+  </si>
 </sst>
 </file>
 
@@ -97,7 +103,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,13 +234,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -587,12 +586,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -917,9 +914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDAF4FF0-9CF5-CA4C-9D3A-0D0AC812B596}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -963,10 +958,10 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="5"/>
+      <c r="O1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="3"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
@@ -977,16 +972,16 @@
       </c>
       <c r="C2" s="1">
         <f>E2*F2</f>
-        <v>192</v>
+        <v>165</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>14</v>
@@ -1008,12 +1003,12 @@
       </c>
       <c r="M2" s="2">
         <f>F2/E2</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" s="5"/>
+        <v>1.3636363636363635</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="3"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -1024,16 +1019,16 @@
       </c>
       <c r="C3" s="1">
         <f t="shared" ref="C3:C7" si="0">E3*F3</f>
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>14</v>
@@ -1054,8 +1049,8 @@
         <v>2</v>
       </c>
       <c r="M3" s="2">
-        <f t="shared" ref="M3:M7" si="1">F3/E3</f>
-        <v>1.5454545454545454</v>
+        <f t="shared" ref="M3:M6" si="1">F3/E3</f>
+        <v>1.25</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -1067,16 +1062,16 @@
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
@@ -1098,7 +1093,7 @@
       </c>
       <c r="M4" s="2">
         <f t="shared" si="1"/>
-        <v>1.4166666666666667</v>
+        <v>1.1538461538461537</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -1110,16 +1105,16 @@
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>221</v>
+        <v>176</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>14</v>
@@ -1141,7 +1136,7 @@
       </c>
       <c r="M5" s="2">
         <f t="shared" si="1"/>
-        <v>1.3076923076923077</v>
+        <v>1.4545454545454546</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -1153,16 +1148,16 @@
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>14</v>
@@ -1184,7 +1179,7 @@
       </c>
       <c r="M6" s="2">
         <f t="shared" si="1"/>
-        <v>1.6363636363636365</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -1196,16 +1191,16 @@
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
@@ -1226,8 +1221,8 @@
         <v>2</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" si="1"/>
-        <v>1.5</v>
+        <f>F7/E7</f>
+        <v>1.5454545454545454</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -1239,16 +1234,16 @@
       </c>
       <c r="C8" s="1">
         <f>E8*F8</f>
-        <v>192</v>
+        <v>165</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E8">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
@@ -1270,7 +1265,7 @@
       </c>
       <c r="M8" s="2">
         <f>F8/E8</f>
-        <v>1.3333333333333333</v>
+        <v>1.3636363636363635</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -1282,16 +1277,16 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" ref="C9:C13" si="2">E9*F9</f>
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>
@@ -1312,8 +1307,8 @@
         <v>3</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" ref="M9:M13" si="3">F9/E9</f>
-        <v>1.5454545454545454</v>
+        <f t="shared" ref="M9:M12" si="3">F9/E9</f>
+        <v>1.25</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -1325,16 +1320,16 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" si="2"/>
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F10" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>14</v>
@@ -1356,7 +1351,7 @@
       </c>
       <c r="M10" s="2">
         <f t="shared" si="3"/>
-        <v>1.4166666666666667</v>
+        <v>1.1538461538461537</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -1368,16 +1363,16 @@
       </c>
       <c r="C11" s="1">
         <f t="shared" si="2"/>
-        <v>221</v>
+        <v>176</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F11" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>14</v>
@@ -1399,7 +1394,7 @@
       </c>
       <c r="M11" s="2">
         <f t="shared" si="3"/>
-        <v>1.3076923076923077</v>
+        <v>1.4545454545454546</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -1411,16 +1406,16 @@
       </c>
       <c r="C12" s="1">
         <f t="shared" si="2"/>
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F12" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>14</v>
@@ -1442,7 +1437,7 @@
       </c>
       <c r="M12" s="2">
         <f t="shared" si="3"/>
-        <v>1.6363636363636365</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -1454,16 +1449,16 @@
       </c>
       <c r="C13" s="1">
         <f t="shared" si="2"/>
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>14</v>
@@ -1484,500 +1479,524 @@
         <v>3</v>
       </c>
       <c r="M13" s="2">
-        <f t="shared" si="3"/>
-        <v>1.5</v>
+        <f>F13/E13</f>
+        <v>1.5454545454545454</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="3">
-        <v>192</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="3">
-        <v>12</v>
-      </c>
-      <c r="F14" s="3">
-        <v>16</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="3">
-        <v>1000</v>
-      </c>
-      <c r="J14" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="K14" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="L14" s="3">
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1">
+        <f>E14*F14</f>
+        <v>165</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>15</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L14" s="1">
         <v>4</v>
       </c>
-      <c r="M14" s="4">
-        <v>1.3</v>
+      <c r="M14" s="2">
+        <f>F14/E14</f>
+        <v>1.3636363636363635</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="3">
-        <v>187</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="3">
-        <v>11</v>
-      </c>
-      <c r="F15" s="3">
-        <v>17</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="3">
-        <v>1000</v>
-      </c>
-      <c r="J15" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="K15" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="L15" s="3">
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" ref="C15:C19" si="4">E15*F15</f>
+        <v>180</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1">
+        <v>15</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L15" s="1">
         <v>4</v>
       </c>
-      <c r="M15" s="4">
-        <v>1.5</v>
+      <c r="M15" s="2">
+        <f t="shared" ref="M15:M18" si="5">F15/E15</f>
+        <v>1.25</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="3">
-        <v>204</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="3">
-        <v>12</v>
-      </c>
-      <c r="F16" s="3">
-        <v>17</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="3">
-        <v>1000</v>
-      </c>
-      <c r="J16" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="K16" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="L16" s="3">
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="4"/>
+        <v>195</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1">
+        <v>13</v>
+      </c>
+      <c r="F16" s="1">
+        <v>15</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L16" s="1">
         <v>4</v>
       </c>
-      <c r="M16" s="4">
-        <v>1.4</v>
+      <c r="M16" s="2">
+        <f t="shared" si="5"/>
+        <v>1.1538461538461537</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="3">
-        <v>221</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="3">
-        <v>13</v>
-      </c>
-      <c r="F17" s="3">
-        <v>17</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="3">
-        <v>1000</v>
-      </c>
-      <c r="J17" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="K17" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="L17" s="3">
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="4"/>
+        <v>176</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1">
+        <v>11</v>
+      </c>
+      <c r="F17" s="1">
+        <v>16</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L17" s="1">
         <v>4</v>
       </c>
-      <c r="M17" s="4">
-        <v>1.3</v>
+      <c r="M17" s="2">
+        <f t="shared" si="5"/>
+        <v>1.4545454545454546</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="3">
-        <v>198</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="3">
-        <v>11</v>
-      </c>
-      <c r="F18" s="3">
-        <v>18</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="3">
-        <v>1000</v>
-      </c>
-      <c r="J18" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="K18" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="L18" s="3">
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="4"/>
+        <v>192</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1">
+        <v>16</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L18" s="1">
         <v>4</v>
       </c>
-      <c r="M18" s="4">
-        <v>1.6</v>
+      <c r="M18" s="2">
+        <f t="shared" si="5"/>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="3">
-        <v>216</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="3">
-        <v>12</v>
-      </c>
-      <c r="F19" s="3">
-        <v>18</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="3">
-        <v>1000</v>
-      </c>
-      <c r="J19" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="K19" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="L19" s="3">
+      <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="4"/>
+        <v>187</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1">
+        <v>11</v>
+      </c>
+      <c r="F19" s="1">
+        <v>17</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L19" s="1">
         <v>4</v>
       </c>
-      <c r="M19" s="4">
-        <v>1.5</v>
+      <c r="M19" s="2">
+        <f>F19/E19</f>
+        <v>1.5454545454545454</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="3">
-        <v>192</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="3">
-        <v>12</v>
-      </c>
-      <c r="F20" s="3">
-        <v>16</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="3">
-        <v>1000</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="K20" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="L20" s="3">
+      <c r="B20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="1">
+        <f>E20*F20</f>
+        <v>165</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20">
+        <v>11</v>
+      </c>
+      <c r="F20">
+        <v>15</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L20" s="1">
         <v>5</v>
       </c>
-      <c r="M20" s="4">
-        <v>1.3</v>
+      <c r="M20" s="2">
+        <f>F20/E20</f>
+        <v>1.3636363636363635</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="3">
-        <v>187</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="3">
-        <v>11</v>
-      </c>
-      <c r="F21" s="3">
-        <v>17</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="3">
-        <v>1000</v>
-      </c>
-      <c r="J21" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="K21" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="L21" s="3">
+      <c r="B21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" ref="C21:C25" si="6">E21*F21</f>
+        <v>180</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1">
+        <v>12</v>
+      </c>
+      <c r="F21" s="1">
+        <v>15</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L21" s="1">
         <v>5</v>
       </c>
-      <c r="M21" s="4">
-        <v>1.5</v>
+      <c r="M21" s="2">
+        <f t="shared" ref="M21:M24" si="7">F21/E21</f>
+        <v>1.25</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="3">
-        <v>204</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="3">
-        <v>12</v>
-      </c>
-      <c r="F22" s="3">
-        <v>17</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="3">
-        <v>1000</v>
-      </c>
-      <c r="J22" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="K22" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="L22" s="3">
+      <c r="B22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="6"/>
+        <v>195</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1">
+        <v>13</v>
+      </c>
+      <c r="F22" s="1">
+        <v>15</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L22" s="1">
         <v>5</v>
       </c>
-      <c r="M22" s="4">
-        <v>1.4</v>
+      <c r="M22" s="2">
+        <f t="shared" si="7"/>
+        <v>1.1538461538461537</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="3">
-        <v>221</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="3">
-        <v>13</v>
-      </c>
-      <c r="F23" s="3">
-        <v>17</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="3">
-        <v>1000</v>
-      </c>
-      <c r="J23" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="K23" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="L23" s="3">
+      <c r="B23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="6"/>
+        <v>176</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="1">
+        <v>11</v>
+      </c>
+      <c r="F23" s="1">
+        <v>16</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L23" s="1">
         <v>5</v>
       </c>
-      <c r="M23" s="4">
-        <v>1.3</v>
+      <c r="M23" s="2">
+        <f t="shared" si="7"/>
+        <v>1.4545454545454546</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="3">
-        <v>198</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="3">
-        <v>11</v>
-      </c>
-      <c r="F24" s="3">
-        <v>18</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="3">
-        <v>1000</v>
-      </c>
-      <c r="J24" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="K24" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="L24" s="3">
+      <c r="B24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="6"/>
+        <v>192</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1">
+        <v>12</v>
+      </c>
+      <c r="F24" s="1">
+        <v>16</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L24" s="1">
         <v>5</v>
       </c>
-      <c r="M24" s="4">
-        <v>1.6</v>
+      <c r="M24" s="2">
+        <f t="shared" si="7"/>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="3">
-        <v>216</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="3">
-        <v>12</v>
-      </c>
-      <c r="F25" s="3">
-        <v>18</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" s="3">
-        <v>1000</v>
-      </c>
-      <c r="J25" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="K25" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="L25" s="3">
+      <c r="B25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="6"/>
+        <v>187</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1">
+        <v>11</v>
+      </c>
+      <c r="F25" s="1">
+        <v>17</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L25" s="1">
         <v>5</v>
       </c>
-      <c r="M25" s="4">
-        <v>1.5</v>
+      <c r="M25" s="2">
+        <f>F25/E25</f>
+        <v>1.5454545454545454</v>
       </c>
     </row>
   </sheetData>
@@ -1989,7 +2008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74957D10-B606-B346-83D0-6265410F7092}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2033,10 +2052,10 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="5"/>
+      <c r="P1" s="3"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
@@ -2080,10 +2099,10 @@
         <f>F2/E2</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="5"/>
+      <c r="P2" s="3"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">

</xml_diff>

<commit_message>
Results after 2021-01-12 analysis
</commit_message>
<xml_diff>
--- a/data/somParams/params_SOM.xlsx
+++ b/data/somParams/params_SOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustinkincaid/Google Drive/2_UVM/MansfieldHydro/data/somParams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AA4E94-33A1-5142-B90F-366F420B8F87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7588B67-9B09-C448-A4CE-4DC099ABB05A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="860" windowWidth="22820" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="21">
   <si>
     <t>myRun</t>
   </si>
@@ -93,7 +93,7 @@
     <t>1.3 ratio of cols to rows</t>
   </si>
   <si>
-    <t>175 Vesanto nodes</t>
+    <t>190 Vesanto nodes</t>
   </si>
 </sst>
 </file>
@@ -912,7 +912,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDAF4FF0-9CF5-CA4C-9D3A-0D0AC812B596}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -972,13 +972,13 @@
       </c>
       <c r="C2" s="1">
         <f>E2*F2</f>
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>15</v>
@@ -990,7 +990,7 @@
         <v>15</v>
       </c>
       <c r="I2" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J2" s="1">
         <v>0.05</v>
@@ -999,11 +999,11 @@
         <v>0.01</v>
       </c>
       <c r="L2" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M2" s="2">
         <f>F2/E2</f>
-        <v>1.3636363636363635</v>
+        <v>1.25</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>20</v>
@@ -1018,14 +1018,14 @@
         <v>16</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C7" si="0">E3*F3</f>
-        <v>180</v>
+        <f t="shared" ref="C3:C6" si="0">E3*F3</f>
+        <v>195</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1">
         <v>15</v>
@@ -1037,7 +1037,7 @@
         <v>15</v>
       </c>
       <c r="I3" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J3" s="1">
         <v>0.05</v>
@@ -1046,11 +1046,11 @@
         <v>0.01</v>
       </c>
       <c r="L3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M3" s="2">
         <f t="shared" ref="M3:M6" si="1">F3/E3</f>
-        <v>1.25</v>
+        <v>1.1538461538461537</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -1062,16 +1062,16 @@
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
@@ -1080,7 +1080,7 @@
         <v>15</v>
       </c>
       <c r="I4" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J4" s="1">
         <v>0.05</v>
@@ -1089,11 +1089,11 @@
         <v>0.01</v>
       </c>
       <c r="L4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M4" s="2">
         <f t="shared" si="1"/>
-        <v>1.1538461538461537</v>
+        <v>1.4545454545454546</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -1105,13 +1105,13 @@
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1">
         <v>16</v>
@@ -1123,7 +1123,7 @@
         <v>15</v>
       </c>
       <c r="I5" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J5" s="1">
         <v>0.05</v>
@@ -1132,11 +1132,11 @@
         <v>0.01</v>
       </c>
       <c r="L5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" si="1"/>
-        <v>1.4545454545454546</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -1148,13 +1148,13 @@
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F6" s="1">
         <v>16</v>
@@ -1166,7 +1166,7 @@
         <v>15</v>
       </c>
       <c r="I6" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J6" s="1">
         <v>0.05</v>
@@ -1175,11 +1175,11 @@
         <v>0.01</v>
       </c>
       <c r="L6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M6" s="2">
         <f t="shared" si="1"/>
-        <v>1.3333333333333333</v>
+        <v>1.2307692307692308</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -1190,17 +1190,17 @@
         <v>16</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="0"/>
-        <v>187</v>
+        <f>E7*F7</f>
+        <v>180</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="1">
-        <v>11</v>
-      </c>
-      <c r="F7" s="1">
-        <v>17</v>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
@@ -1209,7 +1209,7 @@
         <v>15</v>
       </c>
       <c r="I7" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J7" s="1">
         <v>0.05</v>
@@ -1218,11 +1218,11 @@
         <v>0.01</v>
       </c>
       <c r="L7" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M7" s="2">
         <f>F7/E7</f>
-        <v>1.5454545454545454</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -1233,16 +1233,16 @@
         <v>16</v>
       </c>
       <c r="C8" s="1">
-        <f>E8*F8</f>
-        <v>165</v>
+        <f t="shared" ref="C8:C11" si="2">E8*F8</f>
+        <v>195</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E8">
-        <v>11</v>
-      </c>
-      <c r="F8">
+      <c r="E8" s="1">
+        <v>13</v>
+      </c>
+      <c r="F8" s="1">
         <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -1252,7 +1252,7 @@
         <v>15</v>
       </c>
       <c r="I8" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J8" s="1">
         <v>0.05</v>
@@ -1264,8 +1264,8 @@
         <v>3</v>
       </c>
       <c r="M8" s="2">
-        <f>F8/E8</f>
-        <v>1.3636363636363635</v>
+        <f t="shared" ref="M8:M11" si="3">F8/E8</f>
+        <v>1.1538461538461537</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -1276,17 +1276,17 @@
         <v>16</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" ref="C9:C13" si="2">E9*F9</f>
-        <v>180</v>
+        <f t="shared" si="2"/>
+        <v>176</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>
@@ -1295,7 +1295,7 @@
         <v>15</v>
       </c>
       <c r="I9" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J9" s="1">
         <v>0.05</v>
@@ -1307,8 +1307,8 @@
         <v>3</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" ref="M9:M12" si="3">F9/E9</f>
-        <v>1.25</v>
+        <f t="shared" si="3"/>
+        <v>1.4545454545454546</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -1320,16 +1320,16 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" si="2"/>
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>14</v>
@@ -1338,7 +1338,7 @@
         <v>15</v>
       </c>
       <c r="I10" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J10" s="1">
         <v>0.05</v>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="M10" s="2">
         <f t="shared" si="3"/>
-        <v>1.1538461538461537</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -1363,13 +1363,13 @@
       </c>
       <c r="C11" s="1">
         <f t="shared" si="2"/>
-        <v>176</v>
+        <v>208</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F11" s="1">
         <v>16</v>
@@ -1381,7 +1381,7 @@
         <v>15</v>
       </c>
       <c r="I11" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J11" s="1">
         <v>0.05</v>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="M11" s="2">
         <f t="shared" si="3"/>
-        <v>1.4545454545454546</v>
+        <v>1.2307692307692308</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -1405,17 +1405,17 @@
         <v>16</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="2"/>
-        <v>192</v>
+        <f>E12*F12</f>
+        <v>180</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12">
         <v>12</v>
       </c>
-      <c r="F12" s="1">
-        <v>16</v>
+      <c r="F12">
+        <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>14</v>
@@ -1424,7 +1424,7 @@
         <v>15</v>
       </c>
       <c r="I12" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J12" s="1">
         <v>0.05</v>
@@ -1433,11 +1433,11 @@
         <v>0.01</v>
       </c>
       <c r="L12" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M12" s="2">
-        <f t="shared" si="3"/>
-        <v>1.3333333333333333</v>
+        <f>F12/E12</f>
+        <v>1.25</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -1448,17 +1448,17 @@
         <v>16</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="2"/>
-        <v>187</v>
+        <f t="shared" ref="C13:C16" si="4">E13*F13</f>
+        <v>195</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F13" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>14</v>
@@ -1467,7 +1467,7 @@
         <v>15</v>
       </c>
       <c r="I13" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J13" s="1">
         <v>0.05</v>
@@ -1476,11 +1476,11 @@
         <v>0.01</v>
       </c>
       <c r="L13" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M13" s="2">
-        <f>F13/E13</f>
-        <v>1.5454545454545454</v>
+        <f t="shared" ref="M13:M16" si="5">F13/E13</f>
+        <v>1.1538461538461537</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -1491,17 +1491,17 @@
         <v>16</v>
       </c>
       <c r="C14" s="1">
-        <f>E14*F14</f>
-        <v>165</v>
+        <f t="shared" si="4"/>
+        <v>176</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>11</v>
       </c>
-      <c r="F14">
-        <v>15</v>
+      <c r="F14" s="1">
+        <v>16</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>14</v>
@@ -1510,7 +1510,7 @@
         <v>15</v>
       </c>
       <c r="I14" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J14" s="1">
         <v>0.05</v>
@@ -1522,8 +1522,8 @@
         <v>4</v>
       </c>
       <c r="M14" s="2">
-        <f>F14/E14</f>
-        <v>1.3636363636363635</v>
+        <f t="shared" si="5"/>
+        <v>1.4545454545454546</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -1534,8 +1534,8 @@
         <v>16</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:C19" si="4">E15*F15</f>
-        <v>180</v>
+        <f t="shared" si="4"/>
+        <v>192</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
@@ -1544,7 +1544,7 @@
         <v>12</v>
       </c>
       <c r="F15" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>14</v>
@@ -1553,7 +1553,7 @@
         <v>15</v>
       </c>
       <c r="I15" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J15" s="1">
         <v>0.05</v>
@@ -1565,8 +1565,8 @@
         <v>4</v>
       </c>
       <c r="M15" s="2">
-        <f t="shared" ref="M15:M18" si="5">F15/E15</f>
-        <v>1.25</v>
+        <f t="shared" si="5"/>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -1578,7 +1578,7 @@
       </c>
       <c r="C16" s="1">
         <f t="shared" si="4"/>
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -1587,7 +1587,7 @@
         <v>13</v>
       </c>
       <c r="F16" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>14</v>
@@ -1596,7 +1596,7 @@
         <v>15</v>
       </c>
       <c r="I16" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J16" s="1">
         <v>0.05</v>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="M16" s="2">
         <f t="shared" si="5"/>
-        <v>1.1538461538461537</v>
+        <v>1.2307692307692308</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -1620,17 +1620,17 @@
         <v>16</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="4"/>
-        <v>176</v>
+        <f>E17*F17</f>
+        <v>180</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="1">
-        <v>11</v>
-      </c>
-      <c r="F17" s="1">
-        <v>16</v>
+      <c r="E17">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>15</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>14</v>
@@ -1639,7 +1639,7 @@
         <v>15</v>
       </c>
       <c r="I17" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J17" s="1">
         <v>0.05</v>
@@ -1651,8 +1651,8 @@
         <v>4</v>
       </c>
       <c r="M17" s="2">
-        <f t="shared" si="5"/>
-        <v>1.4545454545454546</v>
+        <f>F17/E17</f>
+        <v>1.25</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -1663,17 +1663,17 @@
         <v>16</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="4"/>
-        <v>192</v>
+        <f t="shared" ref="C18:C21" si="6">E18*F18</f>
+        <v>195</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E18" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F18" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>14</v>
@@ -1682,7 +1682,7 @@
         <v>15</v>
       </c>
       <c r="I18" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J18" s="1">
         <v>0.05</v>
@@ -1694,8 +1694,8 @@
         <v>4</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" si="5"/>
-        <v>1.3333333333333333</v>
+        <f t="shared" ref="M18:M21" si="7">F18/E18</f>
+        <v>1.1538461538461537</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -1706,8 +1706,8 @@
         <v>16</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="4"/>
-        <v>187</v>
+        <f t="shared" si="6"/>
+        <v>176</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -1716,7 +1716,7 @@
         <v>11</v>
       </c>
       <c r="F19" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>14</v>
@@ -1725,7 +1725,7 @@
         <v>15</v>
       </c>
       <c r="I19" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J19" s="1">
         <v>0.05</v>
@@ -1737,8 +1737,8 @@
         <v>4</v>
       </c>
       <c r="M19" s="2">
-        <f>F19/E19</f>
-        <v>1.5454545454545454</v>
+        <f t="shared" si="7"/>
+        <v>1.4545454545454546</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -1749,17 +1749,17 @@
         <v>16</v>
       </c>
       <c r="C20" s="1">
-        <f>E20*F20</f>
-        <v>165</v>
+        <f t="shared" si="6"/>
+        <v>192</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E20">
-        <v>11</v>
-      </c>
-      <c r="F20">
-        <v>15</v>
+      <c r="E20" s="1">
+        <v>12</v>
+      </c>
+      <c r="F20" s="1">
+        <v>16</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>14</v>
@@ -1768,7 +1768,7 @@
         <v>15</v>
       </c>
       <c r="I20" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J20" s="1">
         <v>0.05</v>
@@ -1777,11 +1777,11 @@
         <v>0.01</v>
       </c>
       <c r="L20" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M20" s="2">
-        <f>F20/E20</f>
-        <v>1.3636363636363635</v>
+        <f t="shared" si="7"/>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -1792,17 +1792,17 @@
         <v>16</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" ref="C21:C25" si="6">E21*F21</f>
-        <v>180</v>
+        <f t="shared" si="6"/>
+        <v>208</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E21" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F21" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>14</v>
@@ -1811,7 +1811,7 @@
         <v>15</v>
       </c>
       <c r="I21" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J21" s="1">
         <v>0.05</v>
@@ -1820,11 +1820,11 @@
         <v>0.01</v>
       </c>
       <c r="L21" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" ref="M21:M24" si="7">F21/E21</f>
-        <v>1.25</v>
+        <f t="shared" si="7"/>
+        <v>1.2307692307692308</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -1835,16 +1835,16 @@
         <v>16</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="6"/>
-        <v>195</v>
+        <f>E22*F22</f>
+        <v>180</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="1">
-        <v>13</v>
-      </c>
-      <c r="F22" s="1">
+      <c r="E22">
+        <v>12</v>
+      </c>
+      <c r="F22">
         <v>15</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -1854,7 +1854,7 @@
         <v>15</v>
       </c>
       <c r="I22" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J22" s="1">
         <v>0.05</v>
@@ -1866,8 +1866,8 @@
         <v>5</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="7"/>
-        <v>1.1538461538461537</v>
+        <f>F22/E22</f>
+        <v>1.25</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -1878,17 +1878,17 @@
         <v>16</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="6"/>
-        <v>176</v>
+        <f t="shared" ref="C23:C26" si="8">E23*F23</f>
+        <v>195</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E23" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F23" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>14</v>
@@ -1897,7 +1897,7 @@
         <v>15</v>
       </c>
       <c r="I23" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J23" s="1">
         <v>0.05</v>
@@ -1909,8 +1909,8 @@
         <v>5</v>
       </c>
       <c r="M23" s="2">
-        <f t="shared" si="7"/>
-        <v>1.4545454545454546</v>
+        <f t="shared" ref="M23:M26" si="9">F23/E23</f>
+        <v>1.1538461538461537</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -1921,14 +1921,14 @@
         <v>16</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" si="6"/>
-        <v>192</v>
+        <f t="shared" si="8"/>
+        <v>176</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E24" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F24" s="1">
         <v>16</v>
@@ -1940,7 +1940,7 @@
         <v>15</v>
       </c>
       <c r="I24" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J24" s="1">
         <v>0.05</v>
@@ -1952,8 +1952,8 @@
         <v>5</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="7"/>
-        <v>1.3333333333333333</v>
+        <f t="shared" si="9"/>
+        <v>1.4545454545454546</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -1964,17 +1964,17 @@
         <v>16</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" si="6"/>
-        <v>187</v>
+        <f t="shared" si="8"/>
+        <v>192</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E25" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F25" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>14</v>
@@ -1983,7 +1983,7 @@
         <v>15</v>
       </c>
       <c r="I25" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J25" s="1">
         <v>0.05</v>
@@ -1995,8 +1995,266 @@
         <v>5</v>
       </c>
       <c r="M25" s="2">
-        <f>F25/E25</f>
-        <v>1.5454545454545454</v>
+        <f t="shared" si="9"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="8"/>
+        <v>208</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1">
+        <v>13</v>
+      </c>
+      <c r="F26" s="1">
+        <v>16</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1500</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L26" s="1">
+        <v>5</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="9"/>
+        <v>1.2307692307692308</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="1">
+        <f>E27*F27</f>
+        <v>180</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27">
+        <v>12</v>
+      </c>
+      <c r="F27">
+        <v>15</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1500</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L27" s="1">
+        <v>5</v>
+      </c>
+      <c r="M27" s="2">
+        <f>F27/E27</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" ref="C28:C31" si="10">E28*F28</f>
+        <v>195</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1">
+        <v>13</v>
+      </c>
+      <c r="F28" s="1">
+        <v>15</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1500</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L28" s="1">
+        <v>5</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" ref="M28:M31" si="11">F28/E28</f>
+        <v>1.1538461538461537</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="10"/>
+        <v>176</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="1">
+        <v>11</v>
+      </c>
+      <c r="F29" s="1">
+        <v>16</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="1">
+        <v>1500</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L29" s="1">
+        <v>5</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="11"/>
+        <v>1.4545454545454546</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="10"/>
+        <v>192</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="1">
+        <v>12</v>
+      </c>
+      <c r="F30" s="1">
+        <v>16</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1500</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L30" s="1">
+        <v>5</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="11"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="10"/>
+        <v>208</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="1">
+        <v>13</v>
+      </c>
+      <c r="F31" s="1">
+        <v>16</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1500</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L31" s="1">
+        <v>5</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="11"/>
+        <v>1.2307692307692308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>